<commit_message>
created router_questions and return check_questions(answers)
</commit_message>
<xml_diff>
--- a/data/brief/briefP/Parents/b_2.0-3.11_I.xlsx
+++ b/data/brief/briefP/Parents/b_2.0-3.11_I.xlsx
@@ -33,7 +33,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -44,6 +44,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -77,13 +83,13 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -420,37 +426,37 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="3">
         <v>81</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="3">
         <v>104</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="3">
         <v>80</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="3">
         <v>102</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="3">
         <v>79</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="3">
         <v>101</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="3">
         <v>78</v>
       </c>
@@ -462,7 +468,7 @@
         <v>100</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="3">
         <v>77</v>
       </c>
@@ -474,7 +480,7 @@
         <v>98</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="3">
         <v>76</v>
       </c>
@@ -486,7 +492,7 @@
         <v>97</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="3">
         <v>75</v>
       </c>
@@ -498,7 +504,7 @@
         <v>96</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="3">
         <v>74</v>
       </c>
@@ -510,7 +516,7 @@
         <v>94</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="3">
         <v>73</v>
       </c>
@@ -522,7 +528,7 @@
         <v>93</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="3">
         <v>72</v>
       </c>
@@ -534,7 +540,7 @@
         <v>92</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="3">
         <v>71</v>
       </c>
@@ -546,7 +552,7 @@
         <v>91</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="3">
         <v>70</v>
       </c>
@@ -558,7 +564,7 @@
         <v>89</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="3">
         <v>69</v>
       </c>
@@ -570,7 +576,7 @@
         <v>88</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="3">
         <v>68</v>
       </c>
@@ -582,7 +588,7 @@
         <v>87</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="3">
         <v>67</v>
       </c>
@@ -594,7 +600,7 @@
         <v>85</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="3">
         <v>66</v>
       </c>
@@ -606,7 +612,7 @@
         <v>84</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="3">
         <v>65</v>
       </c>
@@ -618,7 +624,7 @@
         <v>83</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="3">
         <v>64</v>
       </c>
@@ -630,7 +636,7 @@
         <v>81</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="3">
         <v>63</v>
       </c>
@@ -642,7 +648,7 @@
         <v>80</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="3">
         <v>62</v>
       </c>
@@ -654,7 +660,7 @@
         <v>79</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="3">
         <v>61</v>
       </c>
@@ -666,7 +672,7 @@
         <v>77</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="3">
         <v>60</v>
       </c>
@@ -680,7 +686,7 @@
         <v>76</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="3">
         <v>59</v>
       </c>
@@ -694,7 +700,7 @@
         <v>75</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="3">
         <v>58</v>
       </c>
@@ -708,7 +714,7 @@
         <v>74</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="3">
         <v>57</v>
       </c>
@@ -722,7 +728,7 @@
         <v>72</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="3">
         <v>56</v>
       </c>
@@ -736,7 +742,7 @@
         <v>71</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="3">
         <v>55</v>
       </c>
@@ -1152,67 +1158,67 @@
       <c r="C57" s="3">
         <v>43</v>
       </c>
-      <c r="D57" s="2"/>
+      <c r="D57" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
       <c r="A58" s="3">
         <v>25</v>
       </c>
-      <c r="B58" s="2"/>
+      <c r="B58" s="1"/>
       <c r="C58" s="3">
         <v>42</v>
       </c>
-      <c r="D58" s="2"/>
+      <c r="D58" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
       <c r="A59" s="3">
         <v>24</v>
       </c>
-      <c r="B59" s="2"/>
+      <c r="B59" s="1"/>
       <c r="C59" s="3">
         <v>40</v>
       </c>
-      <c r="D59" s="2"/>
+      <c r="D59" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
       <c r="A60" s="3">
         <v>23</v>
       </c>
-      <c r="B60" s="2"/>
+      <c r="B60" s="1"/>
       <c r="C60" s="3">
         <v>39</v>
       </c>
-      <c r="D60" s="2"/>
+      <c r="D60" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
       <c r="A61" s="3">
         <v>22</v>
       </c>
-      <c r="B61" s="2"/>
+      <c r="B61" s="1"/>
       <c r="C61" s="3">
         <v>37</v>
       </c>
-      <c r="D61" s="2"/>
+      <c r="D61" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
       <c r="A62" s="3">
         <v>21</v>
       </c>
-      <c r="B62" s="2"/>
+      <c r="B62" s="1"/>
       <c r="C62" s="3">
         <v>36</v>
       </c>
-      <c r="D62" s="2"/>
+      <c r="D62" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
       <c r="A63" s="3">
         <v>20</v>
       </c>
-      <c r="B63" s="2"/>
+      <c r="B63" s="1"/>
       <c r="C63" s="3">
         <v>35</v>
       </c>
-      <c r="D63" s="2"/>
+      <c r="D63" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>